<commit_message>
updated results.xlsx with reduction data
</commit_message>
<xml_diff>
--- a/p6_openCL/results.xlsx
+++ b/p6_openCL/results.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rabbit" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="DGX" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="DGX - first" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="DGX - reduction" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="38">
   <si>
     <t xml:space="preserve">PrintInfo:</t>
   </si>
@@ -127,6 +128,15 @@
   </si>
   <si>
     <t xml:space="preserve">Device Maximum Clock Frequency = 1530 MHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GigaMult-ReductionsPerSecond</t>
   </si>
 </sst>
 </file>
@@ -2621,8 +2631,8 @@
   </sheetPr>
   <dimension ref="A1:P137"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q19" activeCellId="0" sqref="Q19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6250,4 +6260,1206 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L57"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.16"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>523776</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>523776</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>523776</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>523776</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>2096128</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>2096128</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>2096128</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>2096128</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>4096</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>8386560</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.089</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>4096</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>8386560</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>4096</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>8386560</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0.089</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>4096</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>8386560</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>0.089</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>33550336</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>33550336</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>0.178</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>33550336</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>0.179</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G17" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>33550336</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>134209536</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>0.362</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>134209536</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>0.326</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>134209536</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>0.363</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G21" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>134209536</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>0.323</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G22" s="0" t="n">
+        <v>32768</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>536859328</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>0.722</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G23" s="0" t="n">
+        <v>32768</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>536854528</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>0.733</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G24" s="0" t="n">
+        <v>32768</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>536854528</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G25" s="0" t="n">
+        <v>32768</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>536854528</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>0.603</v>
+      </c>
+      <c r="L25" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G26" s="0" t="n">
+        <v>65536</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>2147472000</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>1.161</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G27" s="0" t="n">
+        <v>65536</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>2147467264</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>1.407</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G28" s="0" t="n">
+        <v>65536</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>2147460352</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>1.442</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G29" s="0" t="n">
+        <v>65536</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>2147450880</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>1.489</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G30" s="0" t="n">
+        <v>131072</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>4096</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>8589922816</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>2.544</v>
+      </c>
+      <c r="L30" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G31" s="0" t="n">
+        <v>131072</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>8589918208</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>2.429</v>
+      </c>
+      <c r="L31" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G32" s="0" t="n">
+        <v>131072</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>8589911040</v>
+      </c>
+      <c r="K32" s="0" t="n">
+        <v>2.852</v>
+      </c>
+      <c r="L32" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G33" s="0" t="n">
+        <v>131072</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>8589901824</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <v>2.799</v>
+      </c>
+      <c r="L33" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G34" s="0" t="n">
+        <v>262144</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>34358859776</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>3.786</v>
+      </c>
+      <c r="L34" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G35" s="0" t="n">
+        <v>262144</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>4096</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>34359721984</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>5.073</v>
+      </c>
+      <c r="L35" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G36" s="0" t="n">
+        <v>262144</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>34359713792</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>5.323</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G37" s="0" t="n">
+        <v>262144</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>1024</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>34359705600</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>5.561</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G38" s="0" t="n">
+        <v>524288</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>137438076928</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>2.147</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G39" s="0" t="n">
+        <v>524288</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>137435463680</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>2.214</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G40" s="0" t="n">
+        <v>524288</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>4096</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>137438928896</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>2.368</v>
+      </c>
+      <c r="L40" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G41" s="0" t="n">
+        <v>524288</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>2048</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>137438920704</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>1.971</v>
+      </c>
+      <c r="L41" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G42" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>32768</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>549754961920</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>3.959</v>
+      </c>
+      <c r="L42" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G43" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <v>549752340480</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>4.362</v>
+      </c>
+      <c r="L43" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G44" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <v>549741920256</v>
+      </c>
+      <c r="K44" s="0" t="n">
+        <v>4.568</v>
+      </c>
+      <c r="L44" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G45" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>4096</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <v>549755781120</v>
+      </c>
+      <c r="K45" s="0" t="n">
+        <v>3.687</v>
+      </c>
+      <c r="L45" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G46" s="0" t="n">
+        <v>2097152</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>65536</v>
+      </c>
+      <c r="J46" s="0" t="n">
+        <v>2199022469120</v>
+      </c>
+      <c r="K46" s="0" t="n">
+        <v>6.451</v>
+      </c>
+      <c r="L46" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G47" s="0" t="n">
+        <v>2097152</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>32768</v>
+      </c>
+      <c r="J47" s="0" t="n">
+        <v>2199019847680</v>
+      </c>
+      <c r="K47" s="0" t="n">
+        <v>7.753</v>
+      </c>
+      <c r="L47" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G48" s="0" t="n">
+        <v>2097152</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="J48" s="0" t="n">
+        <v>2199009361920</v>
+      </c>
+      <c r="K48" s="0" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="L48" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G49" s="0" t="n">
+        <v>2097152</v>
+      </c>
+      <c r="H49" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>8192</v>
+      </c>
+      <c r="J49" s="0" t="n">
+        <v>2198967681024</v>
+      </c>
+      <c r="K49" s="0" t="n">
+        <v>8.412</v>
+      </c>
+      <c r="L49" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G50" s="0" t="n">
+        <v>4194304</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>131072</v>
+      </c>
+      <c r="J50" s="0" t="n">
+        <v>8796092497920</v>
+      </c>
+      <c r="K50" s="0" t="n">
+        <v>9.219</v>
+      </c>
+      <c r="L50" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G51" s="0" t="n">
+        <v>4194304</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <v>65536</v>
+      </c>
+      <c r="J51" s="0" t="n">
+        <v>8796089876480</v>
+      </c>
+      <c r="K51" s="0" t="n">
+        <v>12.112</v>
+      </c>
+      <c r="L51" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G52" s="0" t="n">
+        <v>4194304</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>32768</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>8796079390720</v>
+      </c>
+      <c r="K52" s="0" t="n">
+        <v>14.317</v>
+      </c>
+      <c r="L52" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G53" s="0" t="n">
+        <v>4194304</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>16384</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <v>8796037447680</v>
+      </c>
+      <c r="K53" s="0" t="n">
+        <v>14.265</v>
+      </c>
+      <c r="L53" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G54" s="0" t="n">
+        <v>8388608</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>262144</v>
+      </c>
+      <c r="J54" s="0" t="n">
+        <v>35184887988224</v>
+      </c>
+      <c r="K54" s="0" t="n">
+        <v>11.345</v>
+      </c>
+      <c r="L54" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G55" s="0" t="n">
+        <v>8388608</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>131072</v>
+      </c>
+      <c r="J55" s="0" t="n">
+        <v>35184369991680</v>
+      </c>
+      <c r="K55" s="0" t="n">
+        <v>15.659</v>
+      </c>
+      <c r="L55" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G56" s="0" t="n">
+        <v>8388608</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <v>128</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <v>65536</v>
+      </c>
+      <c r="J56" s="0" t="n">
+        <v>35184359505920</v>
+      </c>
+      <c r="K56" s="0" t="n">
+        <v>19.186</v>
+      </c>
+      <c r="L56" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G57" s="0" t="n">
+        <v>8388608</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <v>32768</v>
+      </c>
+      <c r="J57" s="0" t="n">
+        <v>35184317562880</v>
+      </c>
+      <c r="K57" s="0" t="n">
+        <v>20.364</v>
+      </c>
+      <c r="L57" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>